<commit_message>
add metadata for fire history csv files
</commit_message>
<xml_diff>
--- a/ExportedData/states_burned_lakes.xlsx
+++ b/ExportedData/states_burned_lakes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Alabama</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>% burned lakes wildfire</t>
+  </si>
+  <si>
+    <t>% US lakes ≥ 4 ha</t>
   </si>
 </sst>
 </file>
@@ -1032,30 +1035,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="4" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1081,22 +1086,25 @@
         <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1125,22 +1133,25 @@
         <v>1</v>
       </c>
       <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
         <v>20</v>
       </c>
-      <c r="L2" s="4">
+      <c r="K2" s="4">
         <f>D2/C2</f>
         <v>0.95176848874598075</v>
       </c>
-      <c r="M2" s="4">
+      <c r="L2" s="4">
         <f>E2/C2</f>
         <v>2.2508038585209004E-2</v>
       </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M2" s="4">
+        <f>B2/137465</f>
+        <v>7.0126941403266287E-3</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1169,22 +1180,25 @@
         <v>2</v>
       </c>
       <c r="J3" s="3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
         <v>5</v>
       </c>
-      <c r="L3" s="4">
+      <c r="K3" s="4">
         <f>D3/C3</f>
         <v>0.85</v>
       </c>
-      <c r="M3" s="4">
+      <c r="L3" s="4">
         <f>E3/C3</f>
         <v>0.17</v>
       </c>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M3" s="4">
+        <f>B3/137465</f>
+        <v>2.7061433819517695E-3</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1210,25 +1224,28 @@
         <v>0.150776053215078</v>
       </c>
       <c r="I4" s="3">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3">
-        <v>21</v>
-      </c>
-      <c r="K4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="4">
+      <c r="K4" s="4">
         <f>D4/C4</f>
         <v>0.15289256198347106</v>
       </c>
-      <c r="M4" s="4">
+      <c r="L4" s="4">
         <f>E4/C4</f>
         <v>0.56198347107438018</v>
       </c>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M4" s="4">
+        <f>B4/137465</f>
+        <v>1.3123340486669334E-2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1254,25 +1271,28 @@
         <v>4.4619422572178498E-2</v>
       </c>
       <c r="I5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="3">
-        <v>3</v>
-      </c>
-      <c r="K5" s="3">
         <v>6</v>
       </c>
-      <c r="L5" s="4">
+      <c r="K5" s="4">
         <f>D5/C5</f>
         <v>0.88172043010752688</v>
       </c>
-      <c r="M5" s="4">
+      <c r="L5" s="4">
         <f>E5/C5</f>
         <v>0.18279569892473119</v>
       </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M5" s="4">
+        <f>B5/137465</f>
+        <v>2.7716145928054414E-3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1298,25 +1318,28 @@
         <v>9.4184200079396596E-2</v>
       </c>
       <c r="I6" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J6" s="3">
-        <v>10</v>
-      </c>
-      <c r="K6" s="3">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
+      <c r="K6" s="4">
         <f>D6/C6</f>
         <v>0.52842983828899326</v>
       </c>
-      <c r="M6" s="4">
+      <c r="L6" s="4">
         <f>E6/C6</f>
         <v>0.49504434011476267</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M6" s="4">
+        <f>B6/137465</f>
+        <v>7.32986578401775E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1342,25 +1365,28 @@
         <v>1.7344497607655499E-2</v>
       </c>
       <c r="I7" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J7" s="3">
-        <v>4</v>
-      </c>
-      <c r="K7" s="3">
         <v>15</v>
       </c>
-      <c r="L7" s="4">
+      <c r="K7" s="4">
         <f>D7/C7</f>
         <v>0.93357933579335795</v>
       </c>
-      <c r="M7" s="4">
+      <c r="L7" s="4">
         <f>E7/C7</f>
         <v>0.1070110701107011</v>
       </c>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M7" s="4">
+        <f>B7/137465</f>
+        <v>1.2163096060815481E-2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1386,25 +1412,28 @@
         <v>3.0326004548900699E-2</v>
       </c>
       <c r="I8" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J8" s="3">
         <v>8</v>
       </c>
-      <c r="K8" s="3">
-        <v>8</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="K8" s="4">
         <f>D8/C8</f>
         <v>0.68674698795180722</v>
       </c>
-      <c r="M8" s="4">
+      <c r="L8" s="4">
         <f>E8/C8</f>
         <v>0.19277108433734941</v>
       </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M8" s="4">
+        <f>B8/137465</f>
+        <v>1.919033935910959E-2</v>
+      </c>
+      <c r="P8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1430,25 +1459,28 @@
         <v>7.21709006928406E-3</v>
       </c>
       <c r="I9" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J9" s="3">
-        <v>5</v>
-      </c>
-      <c r="K9" s="3">
         <v>21</v>
       </c>
-      <c r="L9" s="4">
+      <c r="K9" s="4">
         <f>D9/C9</f>
         <v>0.95173745173745172</v>
       </c>
-      <c r="M9" s="4">
+      <c r="L9" s="4">
         <f>E9/C9</f>
         <v>4.8262548262548263E-2</v>
       </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M9" s="4">
+        <f>B9/137465</f>
+        <v>2.5199141599679918E-2</v>
+      </c>
+      <c r="P9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1474,25 +1506,28 @@
         <v>6.6261733848702398E-3</v>
       </c>
       <c r="I10" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J10" s="3">
-        <v>7</v>
-      </c>
-      <c r="K10" s="3">
         <v>23</v>
       </c>
-      <c r="L10" s="4">
+      <c r="K10" s="4">
         <f>D10/C10</f>
         <v>0.81782945736434109</v>
       </c>
-      <c r="M10" s="4">
+      <c r="L10" s="4">
         <f>E10/C10</f>
         <v>4.6511627906976744E-2</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M10" s="4">
+        <f>B10/137465</f>
+        <v>1.3174262539555523E-2</v>
+      </c>
+      <c r="P10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1518,25 +1553,28 @@
         <v>1.90839694656489E-3</v>
       </c>
       <c r="I11" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J11" s="3">
-        <v>6</v>
-      </c>
-      <c r="K11" s="3">
         <v>32</v>
       </c>
-      <c r="L11" s="4">
+      <c r="K11" s="4">
         <f>D11/C11</f>
         <v>0.98281786941580751</v>
       </c>
-      <c r="M11" s="4">
+      <c r="L11" s="4">
         <f>E11/C11</f>
         <v>1.3745704467353952E-2</v>
       </c>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M11" s="4">
+        <f>B11/137465</f>
+        <v>1.5247517549921798E-2</v>
+      </c>
+      <c r="P11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1562,25 +1600,28 @@
         <v>2.1289537712895399E-3</v>
       </c>
       <c r="I12" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J12" s="3">
-        <v>9</v>
-      </c>
-      <c r="K12" s="3">
         <v>29</v>
       </c>
-      <c r="L12" s="4">
+      <c r="K12" s="4">
         <f>D12/C12</f>
         <v>0.94054054054054059</v>
       </c>
-      <c r="M12" s="4">
+      <c r="L12" s="4">
         <f>E12/C12</f>
         <v>1.891891891891892E-2</v>
       </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M12" s="4">
+        <f>B12/137465</f>
+        <v>2.3918815698541446E-2</v>
+      </c>
+      <c r="P12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1606,25 +1647,28 @@
         <v>2.4390243902439001E-2</v>
       </c>
       <c r="I13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" s="3">
-        <v>11</v>
-      </c>
-      <c r="K13" s="3">
         <v>10</v>
       </c>
-      <c r="L13" s="4">
+      <c r="K13" s="4">
         <f>D13/C13</f>
         <v>0.89473684210526316</v>
       </c>
-      <c r="M13" s="4">
+      <c r="L13" s="4">
         <f>E13/C13</f>
         <v>0.23684210526315788</v>
       </c>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M13" s="4">
+        <f>B13/137465</f>
+        <v>2.6843196450005457E-3</v>
+      </c>
+      <c r="P13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1653,22 +1697,25 @@
         <v>13</v>
       </c>
       <c r="J14" s="3">
-        <v>13</v>
-      </c>
-      <c r="K14" s="3">
         <v>7</v>
       </c>
-      <c r="L14" s="4">
+      <c r="K14" s="4">
         <f>D14/C14</f>
         <v>0.77358490566037741</v>
       </c>
-      <c r="M14" s="4">
+      <c r="L14" s="4">
         <f>E14/C14</f>
         <v>0.40566037735849059</v>
       </c>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M14" s="4">
+        <f>B14/137465</f>
+        <v>8.4748845160586336E-3</v>
+      </c>
+      <c r="P14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1694,25 +1741,28 @@
         <v>5.7228915662650599E-2</v>
       </c>
       <c r="I15" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J15" s="3">
-        <v>16</v>
-      </c>
-      <c r="K15" s="3">
         <v>4</v>
       </c>
-      <c r="L15" s="4">
+      <c r="K15" s="4">
         <f>D15/C15</f>
         <v>0.72413793103448276</v>
       </c>
-      <c r="M15" s="4">
+      <c r="L15" s="4">
         <f>E15/C15</f>
         <v>0.65517241379310343</v>
       </c>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M15" s="4">
+        <f>B15/137465</f>
+        <v>2.4151602226021168E-3</v>
+      </c>
+      <c r="P15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -1738,25 +1788,28 @@
         <v>1.0504201680672299E-2</v>
       </c>
       <c r="I16" s="3">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J16" s="3">
-        <v>12</v>
-      </c>
-      <c r="K16" s="3">
         <v>17</v>
       </c>
-      <c r="L16" s="4">
+      <c r="K16" s="4">
         <f>D16/C16</f>
         <v>0.87951807228915657</v>
       </c>
-      <c r="M16" s="4">
+      <c r="L16" s="4">
         <f>E16/C16</f>
         <v>0.12048192771084337</v>
       </c>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M16" s="4">
+        <f>B16/137465</f>
+        <v>6.9253991925217325E-3</v>
+      </c>
+      <c r="P16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1782,25 +1835,28 @@
         <v>0</v>
       </c>
       <c r="I17" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J17" s="3">
-        <v>14</v>
-      </c>
-      <c r="K17" s="3">
         <v>37</v>
       </c>
-      <c r="L17" s="4">
+      <c r="K17" s="4">
         <f>D17/C17</f>
         <v>0.88235294117647056</v>
       </c>
+      <c r="L17" s="4">
+        <f>E17/C17</f>
+        <v>0</v>
+      </c>
       <c r="M17" s="4">
-        <f>E17/C17</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B17/137465</f>
+        <v>1.5567599025206416E-3</v>
+      </c>
+      <c r="P17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1826,25 +1882,28 @@
         <v>2.1547156481808501E-2</v>
       </c>
       <c r="I18" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J18" s="3">
-        <v>15</v>
-      </c>
-      <c r="K18" s="3">
         <v>12</v>
       </c>
-      <c r="L18" s="4">
+      <c r="K18" s="4">
         <f>D18/C18</f>
         <v>0.84318181818181814</v>
       </c>
-      <c r="M18" s="4">
+      <c r="L18" s="4">
         <f>E18/C18</f>
         <v>0.27727272727272728</v>
       </c>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M18" s="4">
+        <f>B18/137465</f>
+        <v>4.1188666205943331E-2</v>
+      </c>
+      <c r="P18" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1870,25 +1929,28 @@
         <v>6.0036385688295897E-2</v>
       </c>
       <c r="I19" s="3">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J19" s="3">
-        <v>31</v>
-      </c>
-      <c r="K19" s="3">
         <v>3</v>
       </c>
-      <c r="L19" s="4">
+      <c r="K19" s="4">
         <f>D19/C19</f>
         <v>0.14516129032258066</v>
       </c>
-      <c r="M19" s="4">
+      <c r="L19" s="4">
         <f>E19/C19</f>
         <v>0.79838709677419351</v>
       </c>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M19" s="4">
+        <f>B19/137465</f>
+        <v>1.199578074418943E-2</v>
+      </c>
+      <c r="P19" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
@@ -1914,25 +1976,28 @@
         <v>2.39220318960425E-2</v>
       </c>
       <c r="I20" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J20" s="3">
-        <v>17</v>
-      </c>
-      <c r="K20" s="3">
         <v>11</v>
       </c>
-      <c r="L20" s="4">
+      <c r="K20" s="4">
         <f>D20/C20</f>
         <v>0.81428571428571428</v>
       </c>
-      <c r="M20" s="4">
+      <c r="L20" s="4">
         <f>E20/C20</f>
         <v>0.34714285714285714</v>
       </c>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M20" s="4">
+        <f>B20/137465</f>
+        <v>7.3895173316844281E-2</v>
+      </c>
+      <c r="P20" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1958,25 +2023,28 @@
         <v>5.5813953488372103E-3</v>
       </c>
       <c r="I21" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J21" s="3">
-        <v>18</v>
-      </c>
-      <c r="K21" s="3">
         <v>24</v>
       </c>
-      <c r="L21" s="4">
+      <c r="K21" s="4">
         <f>D21/C21</f>
         <v>0.72463768115942029</v>
       </c>
-      <c r="M21" s="4">
+      <c r="L21" s="4">
         <f>E21/C21</f>
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M21" s="4">
+        <f>B21/137465</f>
+        <v>7.820172407521914E-3</v>
+      </c>
+      <c r="P21" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -2002,25 +2070,28 @@
         <v>1.02645356847616E-2</v>
       </c>
       <c r="I22" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J22" s="3">
-        <v>19</v>
-      </c>
-      <c r="K22" s="3">
         <v>18</v>
       </c>
-      <c r="L22" s="4">
+      <c r="K22" s="4">
         <f>D22/C22</f>
         <v>0.83288043478260865</v>
       </c>
-      <c r="M22" s="4">
+      <c r="L22" s="4">
         <f>E22/C22</f>
         <v>0.20244565217391305</v>
       </c>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M22" s="4">
+        <f>B22/137465</f>
+        <v>0.10559778852798894</v>
+      </c>
+      <c r="P22" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -2046,25 +2117,28 @@
         <v>5.5928411633109597E-4</v>
       </c>
       <c r="I23" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J23" s="3">
-        <v>20</v>
-      </c>
-      <c r="K23" s="3">
         <v>36</v>
       </c>
-      <c r="L23" s="4">
+      <c r="K23" s="4">
         <f>D23/C23</f>
         <v>0.97368421052631582</v>
       </c>
-      <c r="M23" s="4">
+      <c r="L23" s="4">
         <f>E23/C23</f>
         <v>1.3157894736842105E-2</v>
       </c>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M23" s="4">
+        <f>B23/137465</f>
+        <v>1.3006947222929473E-2</v>
+      </c>
+      <c r="P23" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2090,25 +2164,28 @@
         <v>2.9064748201438801E-2</v>
       </c>
       <c r="I24" s="3">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J24" s="3">
-        <v>30</v>
-      </c>
-      <c r="K24" s="3">
         <v>9</v>
       </c>
-      <c r="L24" s="4">
+      <c r="K24" s="4">
         <f>D24/C24</f>
         <v>0.31506849315068491</v>
       </c>
-      <c r="M24" s="4">
+      <c r="L24" s="4">
         <f>E24/C24</f>
         <v>0.69178082191780821</v>
       </c>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M24" s="4">
+        <f>B24/137465</f>
+        <v>2.5279161968501072E-2</v>
+      </c>
+      <c r="P24" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -2134,25 +2211,28 @@
         <v>2.1543985637342899E-2</v>
       </c>
       <c r="I25" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J25" s="3">
-        <v>27</v>
-      </c>
-      <c r="K25" s="3">
         <v>13</v>
       </c>
-      <c r="L25" s="4">
+      <c r="K25" s="4">
         <f>D25/C25</f>
         <v>0.45112781954887216</v>
       </c>
-      <c r="M25" s="4">
+      <c r="L25" s="4">
         <f>E25/C25</f>
         <v>0.5864661654135338</v>
       </c>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M25" s="4">
+        <f>B25/137465</f>
+        <v>5.2675226421270871E-2</v>
+      </c>
+      <c r="P25" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
@@ -2178,25 +2258,28 @@
         <v>2.13204951856946E-2</v>
       </c>
       <c r="I26" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J26" s="3">
-        <v>28</v>
-      </c>
-      <c r="K26" s="3">
         <v>14</v>
       </c>
-      <c r="L26" s="4">
+      <c r="K26" s="4">
         <f>D26/C26</f>
         <v>0.40816326530612246</v>
       </c>
-      <c r="M26" s="4">
+      <c r="L26" s="4">
         <f>E26/C26</f>
         <v>0.63265306122448983</v>
       </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M26" s="4">
+        <f>B26/137465</f>
+        <v>2.1154475684719745E-2</v>
+      </c>
+      <c r="P26" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -2222,25 +2305,28 @@
         <v>7.1174377224199302E-3</v>
       </c>
       <c r="I27" s="3">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J27" s="3">
-        <v>23</v>
-      </c>
-      <c r="K27" s="3">
         <v>22</v>
       </c>
-      <c r="L27" s="4">
+      <c r="K27" s="4">
         <f>D27/C27</f>
         <v>0.78723404255319152</v>
       </c>
-      <c r="M27" s="4">
+      <c r="L27" s="4">
         <f>E27/C27</f>
         <v>0.21276595744680851</v>
       </c>
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M27" s="4">
+        <f>B27/137465</f>
+        <v>1.0220783472156549E-2</v>
+      </c>
+      <c r="P27" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -2266,25 +2352,28 @@
         <v>0</v>
       </c>
       <c r="I28" s="3">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J28" s="3">
-        <v>22</v>
-      </c>
-      <c r="K28" s="3">
         <v>37</v>
       </c>
-      <c r="L28" s="4">
+      <c r="K28" s="4">
         <f>D28/C28</f>
         <v>1</v>
       </c>
+      <c r="L28" s="4">
+        <f>E28/C28</f>
+        <v>0</v>
+      </c>
       <c r="M28" s="4">
-        <f>E28/C28</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B28/137465</f>
+        <v>1.4621903757320045E-3</v>
+      </c>
+      <c r="P28" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -2310,25 +2399,28 @@
         <v>2.3793337865397699E-3</v>
       </c>
       <c r="I29" s="3">
+        <v>24</v>
+      </c>
+      <c r="J29" s="3">
         <v>28</v>
       </c>
-      <c r="J29" s="3">
-        <v>24</v>
-      </c>
-      <c r="K29" s="3">
-        <v>28</v>
-      </c>
-      <c r="L29" s="4">
+      <c r="K29" s="4">
         <f>D29/C29</f>
         <v>0.88157894736842102</v>
       </c>
-      <c r="M29" s="4">
+      <c r="L29" s="4">
         <f>E29/C29</f>
         <v>9.2105263157894732E-2</v>
       </c>
-      <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M29" s="4">
+        <f>B29/137465</f>
+        <v>2.1401811370166952E-2</v>
+      </c>
+      <c r="P29" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
@@ -2354,25 +2446,28 @@
         <v>4.3478260869565201E-3</v>
       </c>
       <c r="I30" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J30" s="3">
         <v>25</v>
       </c>
-      <c r="K30" s="3">
-        <v>25</v>
-      </c>
-      <c r="L30" s="4">
+      <c r="K30" s="4">
         <f>D30/C30</f>
         <v>0.80487804878048785</v>
       </c>
-      <c r="M30" s="4">
+      <c r="L30" s="4">
         <f>E30/C30</f>
         <v>0.1951219512195122</v>
       </c>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M30" s="4">
+        <f>B30/137465</f>
+        <v>2.6770450660168043E-2</v>
+      </c>
+      <c r="P30" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2398,25 +2493,28 @@
         <v>2.8598665395614901E-3</v>
       </c>
       <c r="I31" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J31" s="3">
-        <v>32</v>
-      </c>
-      <c r="K31" s="3">
         <v>27</v>
       </c>
-      <c r="L31" s="4">
+      <c r="K31" s="4">
         <f>D31/C31</f>
         <v>0.43478260869565216</v>
       </c>
-      <c r="M31" s="4">
+      <c r="L31" s="4">
         <f>E31/C31</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M31" s="4">
+        <f>B31/137465</f>
+        <v>7.6310333539446407E-3</v>
+      </c>
+      <c r="P31" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -2442,25 +2540,28 @@
         <v>8.0125687352710102E-3</v>
       </c>
       <c r="I32" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J32" s="3">
-        <v>29</v>
-      </c>
-      <c r="K32" s="3">
         <v>19</v>
       </c>
-      <c r="L32" s="4">
+      <c r="K32" s="4">
         <f>D32/C32</f>
         <v>0.63043478260869568</v>
       </c>
-      <c r="M32" s="4">
+      <c r="L32" s="4">
         <f>E32/C32</f>
         <v>0.36956521739130432</v>
       </c>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M32" s="4">
+        <f>B32/137465</f>
+        <v>4.6302695231513473E-2</v>
+      </c>
+      <c r="P32" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2486,25 +2587,28 @@
         <v>1.4655441222326201E-2</v>
       </c>
       <c r="I33" s="3">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J33" s="3">
-        <v>37</v>
-      </c>
-      <c r="K33" s="3">
         <v>16</v>
       </c>
-      <c r="L33" s="4">
+      <c r="K33" s="4">
         <f>D33/C33</f>
         <v>0.25757575757575757</v>
       </c>
-      <c r="M33" s="4">
+      <c r="L33" s="4">
         <f>E33/C33</f>
         <v>0.71212121212121215</v>
       </c>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M33" s="4">
+        <f>B33/137465</f>
+        <v>2.3329574800858399E-2</v>
+      </c>
+      <c r="P33" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>19</v>
       </c>
@@ -2530,25 +2634,28 @@
         <v>3.4216007140731898E-3</v>
       </c>
       <c r="I34" s="3">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J34" s="3">
         <v>26</v>
       </c>
-      <c r="K34" s="3">
-        <v>26</v>
-      </c>
-      <c r="L34" s="4">
+      <c r="K34" s="4">
         <f>D34/C34</f>
         <v>0.86861313868613144</v>
       </c>
-      <c r="M34" s="4">
+      <c r="L34" s="4">
         <f>E34/C34</f>
         <v>0.16788321167883211</v>
       </c>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M34" s="4">
+        <f>B34/137465</f>
+        <v>4.8899719928709125E-2</v>
+      </c>
+      <c r="P34" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
@@ -2574,25 +2681,28 @@
         <v>1.51057401812689E-3</v>
       </c>
       <c r="I35" s="3">
+        <v>35</v>
+      </c>
+      <c r="J35" s="3">
         <v>34</v>
       </c>
-      <c r="J35" s="3">
-        <v>35</v>
-      </c>
-      <c r="K35" s="3">
-        <v>34</v>
-      </c>
-      <c r="L35" s="4">
+      <c r="K35" s="4">
         <f>D35/C35</f>
         <v>0.7</v>
       </c>
-      <c r="M35" s="4">
+      <c r="L35" s="4">
         <f>E35/C35</f>
         <v>0.15</v>
       </c>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M35" s="4">
+        <f>B35/137465</f>
+        <v>1.4447313861710253E-2</v>
+      </c>
+      <c r="P35" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>46</v>
       </c>
@@ -2618,25 +2728,28 @@
         <v>1.9308125502815799E-3</v>
       </c>
       <c r="I36" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J36" s="3">
-        <v>34</v>
-      </c>
-      <c r="K36" s="3">
         <v>31</v>
       </c>
-      <c r="L36" s="4">
+      <c r="K36" s="4">
         <f>D36/C36</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M36" s="4">
+      <c r="L36" s="4">
         <f>E36/C36</f>
         <v>0.2</v>
       </c>
-      <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M36" s="4">
+        <f>B36/137465</f>
+        <v>4.5211508383952277E-2</v>
+      </c>
+      <c r="P36" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>29</v>
       </c>
@@ -2662,25 +2775,28 @@
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J37" s="3">
-        <v>33</v>
-      </c>
-      <c r="K37" s="3">
         <v>37</v>
       </c>
-      <c r="L37" s="4">
+      <c r="K37" s="4">
         <f>D37/C37</f>
         <v>1</v>
       </c>
+      <c r="L37" s="4">
+        <f>E37/C37</f>
+        <v>0</v>
+      </c>
       <c r="M37" s="4">
-        <f>E37/C37</f>
-        <v>0</v>
-      </c>
-      <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B37/137465</f>
+        <v>3.2488269741388714E-2</v>
+      </c>
+      <c r="P37" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
@@ -2706,25 +2822,28 @@
         <v>1.8438844499078101E-3</v>
       </c>
       <c r="I38" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J38" s="3">
-        <v>36</v>
-      </c>
-      <c r="K38" s="3">
         <v>33</v>
       </c>
-      <c r="L38" s="4">
+      <c r="K38" s="4">
         <f>D38/C38</f>
         <v>0.73333333333333328</v>
       </c>
-      <c r="M38" s="4">
+      <c r="L38" s="4">
         <f>E38/C38</f>
         <v>0.2</v>
       </c>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M38" s="4">
+        <f>B38/137465</f>
+        <v>1.1835740006547121E-2</v>
+      </c>
+      <c r="P38" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -2753,22 +2872,25 @@
         <v>38</v>
       </c>
       <c r="J39" s="3">
-        <v>38</v>
-      </c>
-      <c r="K39" s="3">
         <v>37</v>
       </c>
-      <c r="L39" s="4">
+      <c r="K39" s="4">
         <f>D39/C39</f>
         <v>1</v>
       </c>
+      <c r="L39" s="4">
+        <f>E39/C39</f>
+        <v>0</v>
+      </c>
       <c r="M39" s="4">
-        <f>E39/C39</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B39/137465</f>
+        <v>1.2774160695449751E-2</v>
+      </c>
+      <c r="P39" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>10</v>
       </c>
@@ -2794,25 +2916,28 @@
         <v>1.9317450096587301E-3</v>
       </c>
       <c r="I40" s="3">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J40" s="3">
-        <v>42</v>
-      </c>
-      <c r="K40" s="3">
         <v>30</v>
       </c>
+      <c r="K40" s="4">
+        <f>D40/C40</f>
+        <v>0</v>
+      </c>
       <c r="L40" s="4">
-        <f>D40/C40</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="4">
         <f>E40/C40</f>
         <v>1</v>
       </c>
-      <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M40" s="4">
+        <f>B40/137465</f>
+        <v>2.2594842323500529E-2</v>
+      </c>
+      <c r="P40" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>11</v>
       </c>
@@ -2838,25 +2963,28 @@
         <v>0</v>
       </c>
       <c r="I41" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J41" s="3">
-        <v>39</v>
-      </c>
-      <c r="K41" s="3">
         <v>37</v>
       </c>
-      <c r="L41" s="4">
+      <c r="K41" s="4">
         <f>D41/C41</f>
         <v>1</v>
       </c>
+      <c r="L41" s="4">
+        <f>E41/C41</f>
+        <v>0</v>
+      </c>
       <c r="M41" s="4">
-        <f>E41/C41</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B41/137465</f>
+        <v>2.2929472956752628E-2</v>
+      </c>
+      <c r="P41" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
@@ -2882,25 +3010,28 @@
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J42" s="3">
-        <v>40</v>
-      </c>
-      <c r="K42" s="3">
         <v>37</v>
       </c>
-      <c r="L42" s="4">
+      <c r="K42" s="4">
         <f>D42/C42</f>
         <v>1</v>
       </c>
+      <c r="L42" s="4">
+        <f>E42/C42</f>
+        <v>0</v>
+      </c>
       <c r="M42" s="4">
-        <f>E42/C42</f>
-        <v>0</v>
-      </c>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B42/137465</f>
+        <v>1.1988506165205689E-2</v>
+      </c>
+      <c r="P42" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -2926,25 +3057,28 @@
         <v>0</v>
       </c>
       <c r="I43" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J43" s="3">
-        <v>41</v>
-      </c>
-      <c r="K43" s="3">
         <v>37</v>
       </c>
-      <c r="L43" s="4">
+      <c r="K43" s="4">
         <f>D43/C43</f>
         <v>1</v>
       </c>
+      <c r="L43" s="4">
+        <f>E43/C43</f>
+        <v>0</v>
+      </c>
       <c r="M43" s="4">
-        <f>E43/C43</f>
-        <v>0</v>
-      </c>
-      <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+        <f>B43/137465</f>
+        <v>1.9604990361182847E-2</v>
+      </c>
+      <c r="P43" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
@@ -2970,25 +3104,28 @@
         <v>1.10253583241455E-3</v>
       </c>
       <c r="I44" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J44" s="3">
-        <v>42</v>
-      </c>
-      <c r="K44" s="3">
         <v>35</v>
       </c>
+      <c r="K44" s="4">
+        <f>D44/C44</f>
+        <v>0</v>
+      </c>
       <c r="L44" s="4">
-        <f>D44/C44</f>
-        <v>0</v>
-      </c>
-      <c r="M44" s="4">
         <f>E44/C44</f>
         <v>1</v>
       </c>
-      <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M44" s="4">
+        <f>B44/137465</f>
+        <v>6.5980431382533736E-3</v>
+      </c>
+      <c r="P44" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>32</v>
       </c>
@@ -3014,25 +3151,28 @@
         <v>0</v>
       </c>
       <c r="I45" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J45" s="3">
-        <v>42</v>
-      </c>
-      <c r="K45" s="3">
         <v>37</v>
       </c>
-      <c r="L45" s="4" t="e">
+      <c r="K45" s="4" t="e">
         <f>D45/C45</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M45" s="4" t="e">
+      <c r="L45" s="4" t="e">
         <f>E45/C45</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M45" s="4">
+        <f>B45/137465</f>
+        <v>1.0642709053213545E-2</v>
+      </c>
+      <c r="P45" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>26</v>
       </c>
@@ -3058,25 +3198,28 @@
         <v>0</v>
       </c>
       <c r="I46" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J46" s="3">
-        <v>42</v>
-      </c>
-      <c r="K46" s="3">
         <v>37</v>
       </c>
-      <c r="L46" s="4" t="e">
+      <c r="K46" s="4" t="e">
         <f>D46/C46</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M46" s="4" t="e">
+      <c r="L46" s="4" t="e">
         <f>E46/C46</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M46" s="4">
+        <f>B46/137465</f>
+        <v>8.1402538828065328E-3</v>
+      </c>
+      <c r="P46" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
@@ -3102,25 +3245,28 @@
         <v>0</v>
       </c>
       <c r="I47" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J47" s="3">
-        <v>42</v>
-      </c>
-      <c r="K47" s="3">
         <v>37</v>
       </c>
-      <c r="L47" s="4" t="e">
+      <c r="K47" s="4" t="e">
         <f>D47/C47</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M47" s="4" t="e">
+      <c r="L47" s="4" t="e">
         <f>E47/C47</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M47" s="4">
+        <f>B47/137465</f>
+        <v>5.8705852398792417E-3</v>
+      </c>
+      <c r="P47" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>42</v>
       </c>
@@ -3146,25 +3292,28 @@
         <v>0</v>
       </c>
       <c r="I48" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J48" s="3">
-        <v>42</v>
-      </c>
-      <c r="K48" s="3">
         <v>37</v>
       </c>
-      <c r="L48" s="4" t="e">
+      <c r="K48" s="4" t="e">
         <f>D48/C48</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M48" s="4" t="e">
+      <c r="L48" s="4" t="e">
         <f>E48/C48</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N48" s="3"/>
-    </row>
-    <row r="49" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M48" s="4">
+        <f>B48/137465</f>
+        <v>3.797330229512967E-3</v>
+      </c>
+      <c r="P48" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>36</v>
       </c>
@@ -3190,23 +3339,26 @@
         <v>0</v>
       </c>
       <c r="I49" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J49" s="3">
-        <v>42</v>
-      </c>
-      <c r="K49" s="3">
         <v>37</v>
       </c>
-      <c r="L49" s="4" t="e">
+      <c r="K49" s="4" t="e">
         <f>D49/C49</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M49" s="4" t="e">
+      <c r="L49" s="4" t="e">
         <f>E49/C49</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N49" s="3"/>
+      <c r="M49" s="4">
+        <f>B49/137465</f>
+        <v>1.8331939039028116E-3</v>
+      </c>
+      <c r="P49" s="3">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:N49">

</xml_diff>